<commit_message>
implement class field in frontend
</commit_message>
<xml_diff>
--- a/misc/api-specs.xlsx
+++ b/misc/api-specs.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">post/{username,password}</t>
   </si>
   <si>
-    <t xml:space="preserve">{ exists: Boolean, privilege:”teacher/student/parent”, class }</t>
+    <t xml:space="preserve">{ exists: Boolean, privilege:”teacher/student/parent”, userClass }</t>
   </si>
   <si>
     <t xml:space="preserve">Exists should be true/false,</t>
@@ -247,7 +247,7 @@
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
implement teacher assignment upload class based
</commit_message>
<xml_diff>
--- a/misc/api-specs.xlsx
+++ b/misc/api-specs.xlsx
@@ -94,13 +94,13 @@
     <t xml:space="preserve">{ data: [ {name, maxMarks, description, dueDate, id, text}]}</t>
   </si>
   <si>
-    <t xml:space="preserve">/teachers/assignments/{assignmentName}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post/{file:filename, text}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/students/progress/{studentid}</t>
+    <t xml:space="preserve">/teachers/assignments/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post/{file:filename, text, userClass}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/students/progress/{username}</t>
   </si>
   <si>
     <t xml:space="preserve">{ data: [ {name, grade, description, id}]}</t>
@@ -112,10 +112,10 @@
     <t xml:space="preserve">post/{username, subject-name, max-marks, marks-obtained, description}</t>
   </si>
   <si>
-    <t xml:space="preserve">/parents/progress/{parentid}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/students/attendence/{studentid}</t>
+    <t xml:space="preserve">/parents/progress/{username}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/students/attendence/{username}</t>
   </si>
   <si>
     <t xml:space="preserve">{ data: [ {name, attednece,remarks}]}</t>
@@ -127,10 +127,10 @@
     <t xml:space="preserve">post/{username, attedence, remarks etc}</t>
   </si>
   <si>
-    <t xml:space="preserve">/parents/attendence/{parentid}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/parents/fees/{parentid}</t>
+    <t xml:space="preserve">/parents/attendence/{username}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/parents/fees/{username}</t>
   </si>
   <si>
     <t xml:space="preserve">{ data:  {name, cost, description, id}}</t>
@@ -247,7 +247,7 @@
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
implement real fetch in custom fetch
</commit_message>
<xml_diff>
--- a/misc/api-specs.xlsx
+++ b/misc/api-specs.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">status indicated success of post operation</t>
   </si>
   <si>
-    <t xml:space="preserve">/students/assignments</t>
+    <t xml:space="preserve">/students/assignments/{userClass}</t>
   </si>
   <si>
     <t xml:space="preserve">{ data: [ {name, maxMarks, description, dueDate, id, text}]}</t>
@@ -246,8 +246,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>